<commit_message>
added and completed route for forming excel
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -8,13 +8,14 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="РБ №1" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -25,10 +26,166 @@
     <t>Стоимость</t>
   </si>
   <si>
+    <t xml:space="preserve">Аква Марис БЕБИ для детей 150 мл спрей назальный </t>
+  </si>
+  <si>
+    <t>00000064865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аква Марис Классик 30 мл спрей назальный </t>
+  </si>
+  <si>
+    <t>00000001156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Амоксициллин + клавулановая кислота 500 мг/125  мг № 14 табл п/плён оболоч	 </t>
+  </si>
+  <si>
+    <t>00000100309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Беродуал Н 10 мл 200 доз аэрозоль для ингаляций дозированный </t>
+  </si>
+  <si>
+    <t>00000006539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гроприносин 500 мг № 20 табл </t>
+  </si>
+  <si>
+    <t>00000059306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гроприносин 500 мг № 50 табл </t>
+  </si>
+  <si>
+    <t>00000006688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Диклофенак-Тева 75 мг/2 мл № 5 амп </t>
+  </si>
+  <si>
+    <t>00000001820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зитмак 250 мг № 6 табл п/плён оболоч	 </t>
+  </si>
+  <si>
+    <t>00000005318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кандибиотик 5 мл капли ушные во флаконах </t>
+  </si>
+  <si>
+    <t>00000003068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Линекс № 16 капс </t>
+  </si>
+  <si>
+    <t>00000004301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Магний В6 Эвалар № 30 табл </t>
+  </si>
+  <si>
+    <t>00000078952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Називин 0,025% 10 мл капли </t>
+  </si>
+  <si>
+    <t>00000001144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регидрон пор д/пригот-я раствора д/приема внутрь 18,9 г № 20 пакетики </t>
+  </si>
+  <si>
+    <t>00000005342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Смекта Экспресс 3 гр № 12 порошок </t>
+  </si>
+  <si>
+    <t>00000070258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумамокс 500 мг № 3 табл покрытые оболочкой	 </t>
+  </si>
+  <si>
+    <t>00000004580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Супрастин 25 мг № 20 табл </t>
+  </si>
+  <si>
+    <t>00000002868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Танфлекс 0,15 % 30 мл спрей для горла </t>
+  </si>
+  <si>
+    <t>00000000999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТераФлю порошок со вкусом лимона № 10 пакетики </t>
+  </si>
+  <si>
+    <t>00000001228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тонзилгон® Н 100 мл флакон </t>
+  </si>
+  <si>
+    <t>00000100339</t>
+  </si>
+  <si>
+    <t>Ферталь №15, капс.</t>
+  </si>
+  <si>
+    <t>00000000139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холудексан № 20 капс </t>
+  </si>
+  <si>
+    <t>00000002886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шприц 5 мл BBraun (0,70x30 мм) инъекц. 2х-комп.стер. </t>
+  </si>
+  <si>
+    <t>00000076279</t>
+  </si>
+  <si>
+    <t>Итог:</t>
+  </si>
+  <si>
     <t>Сумма / Процент РБ</t>
   </si>
   <si>
-    <t>Итог:</t>
+    <t>Период</t>
+  </si>
+  <si>
+    <t>Номер договора/ДС</t>
+  </si>
+  <si>
+    <t>Тип скидки</t>
+  </si>
+  <si>
+    <t>Сумма вознаграждения</t>
+  </si>
+  <si>
+    <t>Сумма скидки</t>
+  </si>
+  <si>
+    <t>16.02.2022-16.02.2022</t>
+  </si>
+  <si>
+    <t>999еее</t>
+  </si>
+  <si>
+    <t>Скидка за объем закупа</t>
   </si>
 </sst>
 </file>
@@ -371,20 +528,332 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" s="1" t="s">
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
+      <c r="C2">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>4263</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>2764</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>2988</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22">
+        <v>5653</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>680</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1">
+        <v>55056</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
[bugfix] getting report rb
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -26,6 +26,138 @@
     <t>Стоимость</t>
   </si>
   <si>
+    <t xml:space="preserve">Аква Марис БЕБИ для детей 150 мл спрей назальный </t>
+  </si>
+  <si>
+    <t>00000064865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аква Марис Классик 30 мл спрей назальный </t>
+  </si>
+  <si>
+    <t>00000001156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Амоксициллин + клавулановая кислота 500 мг/125  мг № 14 табл п/плён оболоч	 </t>
+  </si>
+  <si>
+    <t>00000100309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Беродуал Н 10 мл 200 доз аэрозоль для ингаляций дозированный </t>
+  </si>
+  <si>
+    <t>00000006539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гроприносин 500 мг № 20 табл </t>
+  </si>
+  <si>
+    <t>00000059306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гроприносин 500 мг № 50 табл </t>
+  </si>
+  <si>
+    <t>00000006688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Диклофенак-Тева 75 мг/2 мл № 5 амп </t>
+  </si>
+  <si>
+    <t>00000001820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зитмак 250 мг № 6 табл п/плён оболоч	 </t>
+  </si>
+  <si>
+    <t>00000005318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кандибиотик 5 мл капли ушные во флаконах </t>
+  </si>
+  <si>
+    <t>00000003068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Линекс № 16 капс </t>
+  </si>
+  <si>
+    <t>00000004301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Магний В6 Эвалар № 30 табл </t>
+  </si>
+  <si>
+    <t>00000078952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Називин 0,025% 10 мл капли </t>
+  </si>
+  <si>
+    <t>00000001144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регидрон пор д/пригот-я раствора д/приема внутрь 18,9 г № 20 пакетики </t>
+  </si>
+  <si>
+    <t>00000005342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Смекта Экспресс 3 гр № 12 порошок </t>
+  </si>
+  <si>
+    <t>00000070258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумамокс 500 мг № 3 табл покрытые оболочкой	 </t>
+  </si>
+  <si>
+    <t>00000004580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Супрастин 25 мг № 20 табл </t>
+  </si>
+  <si>
+    <t>00000002868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Танфлекс 0,15 % 30 мл спрей для горла </t>
+  </si>
+  <si>
+    <t>00000000999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТераФлю порошок со вкусом лимона № 10 пакетики </t>
+  </si>
+  <si>
+    <t>00000001228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тонзилгон® Н 100 мл флакон </t>
+  </si>
+  <si>
+    <t>00000100339</t>
+  </si>
+  <si>
+    <t>Ферталь №15, капс.</t>
+  </si>
+  <si>
+    <t>00000000139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холудексан № 20 капс </t>
+  </si>
+  <si>
+    <t>00000002886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шприц 5 мл BBraun (0,70x30 мм) инъекц. 2х-комп.стер. </t>
+  </si>
+  <si>
+    <t>00000076279</t>
+  </si>
+  <si>
     <t>Итог:</t>
   </si>
   <si>
@@ -45,6 +177,15 @@
   </si>
   <si>
     <t>Сумма скидки</t>
+  </si>
+  <si>
+    <t>16.02.2022-16.02.2022</t>
+  </si>
+  <si>
+    <t>999еее</t>
+  </si>
+  <si>
+    <t>Скидка за объем закупа</t>
   </si>
 </sst>
 </file>
@@ -390,25 +531,276 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2">
-      <c r="D2" t="s">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2">
+        <v>2462</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>4263</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>2764</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>2988</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22">
+        <v>5653</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>680</v>
+      </c>
+      <c r="D24" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1">
+        <v>55056</v>
+      </c>
+      <c r="D25" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -422,28 +814,43 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4">
-      <c r="D4" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="D3" t="s">
+        <v>47</v>
+      </c>
+      <c r="E3">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[bugfix] froming excel for RB-report
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -26,6 +26,138 @@
     <t>Стоимость</t>
   </si>
   <si>
+    <t xml:space="preserve">Аква Марис БЕБИ для детей 150 мл спрей назальный </t>
+  </si>
+  <si>
+    <t>00000064865</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Аква Марис Классик 30 мл спрей назальный </t>
+  </si>
+  <si>
+    <t>00000001156</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Амоксициллин + клавулановая кислота 500 мг/125  мг № 14 табл п/плён оболоч	 </t>
+  </si>
+  <si>
+    <t>00000100309</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Беродуал Н 10 мл 200 доз аэрозоль для ингаляций дозированный </t>
+  </si>
+  <si>
+    <t>00000006539</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гроприносин 500 мг № 20 табл </t>
+  </si>
+  <si>
+    <t>00000059306</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Гроприносин 500 мг № 50 табл </t>
+  </si>
+  <si>
+    <t>00000006688</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Диклофенак-Тева 75 мг/2 мл № 5 амп </t>
+  </si>
+  <si>
+    <t>00000001820</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Зитмак 250 мг № 6 табл п/плён оболоч	 </t>
+  </si>
+  <si>
+    <t>00000005318</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Кандибиотик 5 мл капли ушные во флаконах </t>
+  </si>
+  <si>
+    <t>00000003068</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Линекс № 16 капс </t>
+  </si>
+  <si>
+    <t>00000004301</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Магний В6 Эвалар № 30 табл </t>
+  </si>
+  <si>
+    <t>00000078952</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Називин 0,025% 10 мл капли </t>
+  </si>
+  <si>
+    <t>00000001144</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Регидрон пор д/пригот-я раствора д/приема внутрь 18,9 г № 20 пакетики </t>
+  </si>
+  <si>
+    <t>00000005342</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Смекта Экспресс 3 гр № 12 порошок </t>
+  </si>
+  <si>
+    <t>00000070258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Сумамокс 500 мг № 3 табл покрытые оболочкой	 </t>
+  </si>
+  <si>
+    <t>00000004580</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Супрастин 25 мг № 20 табл </t>
+  </si>
+  <si>
+    <t>00000002868</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Танфлекс 0,15 % 30 мл спрей для горла </t>
+  </si>
+  <si>
+    <t>00000000999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ТераФлю порошок со вкусом лимона № 10 пакетики </t>
+  </si>
+  <si>
+    <t>00000001228</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Тонзилгон® Н 100 мл флакон </t>
+  </si>
+  <si>
+    <t>00000100339</t>
+  </si>
+  <si>
+    <t>Ферталь №15, капс.</t>
+  </si>
+  <si>
+    <t>00000000139</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Холудексан № 20 капс </t>
+  </si>
+  <si>
+    <t>00000002886</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Шприц 5 мл BBraun (0,70x30 мм) инъекц. 2х-комп.стер. </t>
+  </si>
+  <si>
+    <t>00000076279</t>
+  </si>
+  <si>
     <t>Итог:</t>
   </si>
   <si>
@@ -47,10 +179,10 @@
     <t>Сумма скидки</t>
   </si>
   <si>
-    <t>10.02.2022-18.02.2022</t>
-  </si>
-  <si>
-    <t>3546980</t>
+    <t>23.02.2022-23.02.2022</t>
+  </si>
+  <si>
+    <t>2500800DLR</t>
   </si>
   <si>
     <t>Скидка за объем закупа</t>
@@ -399,25 +531,276 @@
       <c r="D1" s="1"/>
     </row>
     <row r="2">
-      <c r="D2" s="1" t="s">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
+      <c r="C2">
+        <v>2462</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1">
-        <v>0</v>
-      </c>
-      <c r="D3" s="1">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3">
+        <v>2459</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4">
+        <v>3319</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5">
+        <v>4263</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7">
+        <v>3180</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8">
+        <v>2565</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9">
+        <v>3321</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10">
+        <v>3001</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11">
+        <v>2764</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12">
+        <v>1380</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>25</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13">
+        <v>872</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14">
+        <v>815</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B15" t="s">
+        <v>30</v>
+      </c>
+      <c r="C15">
+        <v>1912</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>32</v>
+      </c>
+      <c r="C16">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17">
+        <v>1786</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+      <c r="C18">
+        <v>1841</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>37</v>
+      </c>
+      <c r="B19" t="s">
+        <v>38</v>
+      </c>
+      <c r="C19">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" t="s">
+        <v>40</v>
+      </c>
+      <c r="C20">
+        <v>2988</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21">
+        <v>3590</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22">
+        <v>5653</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+      <c r="C23">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24">
+        <v>680</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1">
+        <v>55056</v>
+      </c>
+      <c r="D25" s="1">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A25:B25"/>
   </mergeCells>
 </worksheet>
 </file>
@@ -431,33 +814,33 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>5</v>
+        <v>49</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>6</v>
+        <v>50</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>9</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="D2">
-        <v>750000</v>
+        <v>10000</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -465,7 +848,7 @@
     </row>
     <row r="3">
       <c r="D3" s="1" t="s">
-        <v>3</v>
+        <v>47</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>

</xml_diff>

<commit_message>
added count of product in forming excel
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -26,6 +26,12 @@
     <t>Стоимость</t>
   </si>
   <si>
+    <t>Количество</t>
+  </si>
+  <si>
+    <t>Итог:</t>
+  </si>
+  <si>
     <t xml:space="preserve">Аква Марис БЕБИ для детей 150 мл спрей назальный </t>
   </si>
   <si>
@@ -156,9 +162,6 @@
   </si>
   <si>
     <t>00000076279</t>
-  </si>
-  <si>
-    <t>Итог:</t>
   </si>
   <si>
     <t>Сумма / Процент РБ</t>
@@ -528,280 +531,422 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1"/>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C2">
         <v>2462</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>2462</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <v>2459</v>
       </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>2459</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C4">
         <v>3319</v>
       </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>3319</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C5">
         <v>4263</v>
       </c>
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>4263</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C6">
         <v>2268</v>
       </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>2268</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>3180</v>
       </c>
+      <c r="D7">
+        <v>30</v>
+      </c>
+      <c r="E7">
+        <v>95400</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B8" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C8">
         <v>2565</v>
       </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2565</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C9">
         <v>3321</v>
       </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>3321</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B10" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C10">
         <v>3001</v>
       </c>
+      <c r="D10">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>3001</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C11">
         <v>2764</v>
       </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2764</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B12" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C12">
         <v>1380</v>
       </c>
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>1380</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B13" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C13">
         <v>872</v>
       </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>872</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B14" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C14">
         <v>815</v>
       </c>
+      <c r="D14">
+        <v>5</v>
+      </c>
+      <c r="E14">
+        <v>4075</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C15">
         <v>1912</v>
       </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1912</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <v>1605</v>
       </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1605</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="C17">
         <v>1786</v>
       </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1786</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <v>1841</v>
       </c>
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>1841</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="C19">
         <v>2162</v>
       </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>2162</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>2988</v>
       </c>
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>2988</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C21">
         <v>3590</v>
       </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>3590</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C22">
         <v>5653</v>
       </c>
+      <c r="D22">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>5653</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C23">
         <v>170</v>
       </c>
+      <c r="D23">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>850</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C24">
         <v>680</v>
       </c>
-      <c r="D24" s="1" t="s">
-        <v>48</v>
+      <c r="D24">
+        <v>20</v>
+      </c>
+      <c r="E24">
+        <v>13600</v>
+      </c>
+      <c r="F24" s="1" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="1" t="s">
-        <v>47</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="1">
-        <v>55056</v>
-      </c>
-      <c r="D25" s="1">
-        <v>0</v>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="1">
+        <v>164136</v>
+      </c>
+      <c r="F25" s="1">
+        <v>5000</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A25:B25"/>
-  </mergeCells>
 </worksheet>
 </file>
 
@@ -814,44 +959,44 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D2">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="E2">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
     <row r="3">
       <c r="D3" s="1" t="s">
-        <v>47</v>
+        <v>4</v>
       </c>
       <c r="E3" s="1">
-        <v>0</v>
+        <v>5000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed bug with forming RB #2
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -162,9 +162,6 @@
   </si>
   <si>
     <t>00000076279</t>
-  </si>
-  <si>
-    <t>Сумма / Процент РБ</t>
   </si>
   <si>
     <t>Период</t>
@@ -928,9 +925,6 @@
       <c r="E24">
         <v>13600</v>
       </c>
-      <c r="F24" s="1" t="s">
-        <v>49</v>
-      </c>
     </row>
     <row r="25">
       <c r="A25" s="1"/>
@@ -941,9 +935,6 @@
       </c>
       <c r="E25" s="1">
         <v>164136</v>
-      </c>
-      <c r="F25" s="1">
-        <v>5000</v>
       </c>
     </row>
   </sheetData>
@@ -959,30 +950,30 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
         <v>55</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>56</v>
-      </c>
-      <c r="C2" t="s">
-        <v>57</v>
       </c>
       <c r="D2">
         <v>5000</v>

</xml_diff>

<commit_message>
added for RB #3
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -9,13 +9,14 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Скидка за объем закупа" sheetId="2" r:id="rId5"/>
+    <sheet name="Скидка  на группы товаров" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -179,13 +180,31 @@
     <t>Сумма скидки</t>
   </si>
   <si>
-    <t>23.02.2022-23.02.2022</t>
+    <t>01.03.2022-01.01.2022</t>
   </si>
   <si>
     <t>2500800DLR</t>
   </si>
   <si>
     <t>Скидка за объем закупа</t>
+  </si>
+  <si>
+    <t>Код товара</t>
+  </si>
+  <si>
+    <t>План закупа</t>
+  </si>
+  <si>
+    <t>Скидка %</t>
+  </si>
+  <si>
+    <t>Скидка  на группы товаров</t>
+  </si>
+  <si>
+    <t>00000045698</t>
+  </si>
+  <si>
+    <t>00000053058</t>
   </si>
 </sst>
 </file>
@@ -992,4 +1011,115 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2">
+        <v>500</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>295.44</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B3" t="s">
+        <v>55</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
+      <c r="G3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4">
+        <v>1500</v>
+      </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="F5" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="1">
+        <v>295.44</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bugfix with RB #3
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Скидка за объем закупа" sheetId="2" r:id="rId5"/>
-    <sheet name="Скидка  на группы товаров" sheetId="3" r:id="rId6"/>
+    <sheet name="Скидка за выполнение плана заку" sheetId="3" r:id="rId6"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
@@ -198,7 +198,7 @@
     <t>Скидка %</t>
   </si>
   <si>
-    <t>Скидка  на группы товаров</t>
+    <t>Скидка за выполнение плана закупа по препаратам</t>
   </si>
   <si>
     <t>00000045698</t>

</xml_diff>

<commit_message>
[add] added mocks for forming all RB types
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="true"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
+    <workbookView windowWidth="25460" windowHeight="12200" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Скидка за объем закупа" sheetId="2" r:id="rId5"/>
-    <sheet name="Скидка за выполнение плана заку" sheetId="3" r:id="rId6"/>
+    <sheet name="Скидка за объем закупа" sheetId="2" r:id="rId2"/>
+    <sheet name="Скидка за выполнение плана заку" sheetId="3" r:id="rId3"/>
+    <sheet name="Скидка за представленность" sheetId="4" r:id="rId4"/>
+    <sheet name="Скидка на РБ от закупа продукци" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65">
   <si>
     <t>Номенклатура</t>
   </si>
@@ -205,21 +207,184 @@
   </si>
   <si>
     <t>00000053058</t>
+  </si>
+  <si>
+    <t>Скидка за представленность</t>
+  </si>
+  <si>
+    <t>Скидка за прСкидка на РБ от закупа продукциедставленность</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -229,10 +394,197 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5DEB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -255,21 +607,313 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyAlignment="false">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -316,7 +960,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -351,7 +995,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -525,19 +1169,28 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E25"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="72.78125" customWidth="1"/>
+    <col min="2" max="2" width="15.5625" customWidth="1"/>
+    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="11.375" customWidth="1"/>
+    <col min="5" max="5" width="7.5" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -554,7 +1207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -571,7 +1224,7 @@
         <v>2462</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:5">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -588,7 +1241,7 @@
         <v>2459</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:5">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -605,7 +1258,7 @@
         <v>3319</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:5">
       <c r="A5" t="s">
         <v>11</v>
       </c>
@@ -622,7 +1275,7 @@
         <v>4263</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:5">
       <c r="A6" t="s">
         <v>13</v>
       </c>
@@ -639,7 +1292,7 @@
         <v>2268</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:5">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -656,7 +1309,7 @@
         <v>95400</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:5">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -673,7 +1326,7 @@
         <v>2565</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:5">
       <c r="A9" t="s">
         <v>19</v>
       </c>
@@ -690,7 +1343,7 @@
         <v>3321</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:5">
       <c r="A10" t="s">
         <v>21</v>
       </c>
@@ -707,7 +1360,7 @@
         <v>3001</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:5">
       <c r="A11" t="s">
         <v>23</v>
       </c>
@@ -724,7 +1377,7 @@
         <v>2764</v>
       </c>
     </row>
-    <row r="12">
+    <row r="12" spans="1:5">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -741,7 +1394,7 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:5">
       <c r="A13" t="s">
         <v>27</v>
       </c>
@@ -758,7 +1411,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:5">
       <c r="A14" t="s">
         <v>29</v>
       </c>
@@ -775,7 +1428,7 @@
         <v>4075</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:5">
       <c r="A15" t="s">
         <v>31</v>
       </c>
@@ -792,7 +1445,7 @@
         <v>1912</v>
       </c>
     </row>
-    <row r="16">
+    <row r="16" spans="1:5">
       <c r="A16" t="s">
         <v>33</v>
       </c>
@@ -809,7 +1462,7 @@
         <v>1605</v>
       </c>
     </row>
-    <row r="17">
+    <row r="17" spans="1:5">
       <c r="A17" t="s">
         <v>35</v>
       </c>
@@ -826,7 +1479,7 @@
         <v>1786</v>
       </c>
     </row>
-    <row r="18">
+    <row r="18" spans="1:5">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -843,7 +1496,7 @@
         <v>1841</v>
       </c>
     </row>
-    <row r="19">
+    <row r="19" spans="1:5">
       <c r="A19" t="s">
         <v>39</v>
       </c>
@@ -860,7 +1513,7 @@
         <v>2162</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:5">
       <c r="A20" t="s">
         <v>41</v>
       </c>
@@ -877,7 +1530,7 @@
         <v>2988</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:5">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -894,7 +1547,7 @@
         <v>3590</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:5">
       <c r="A22" t="s">
         <v>45</v>
       </c>
@@ -911,7 +1564,7 @@
         <v>5653</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:5">
       <c r="A23" t="s">
         <v>47</v>
       </c>
@@ -928,7 +1581,7 @@
         <v>850</v>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:5">
       <c r="A24" t="s">
         <v>47</v>
       </c>
@@ -945,7 +1598,7 @@
         <v>13600</v>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:5">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -957,17 +1610,23 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -984,7 +1643,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1001,7 +1660,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="4:5">
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
@@ -1010,17 +1669,32 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:G5"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="6"/>
+  <cols>
+    <col min="1" max="1" width="21.25" customWidth="1"/>
+    <col min="2" max="2" width="19.0625" customWidth="1"/>
+    <col min="3" max="3" width="43.484375" customWidth="1"/>
+    <col min="4" max="4" width="12.75" customWidth="1"/>
+    <col min="5" max="5" width="11.875" customWidth="1"/>
+    <col min="6" max="6" width="9.8125" customWidth="1"/>
+    <col min="7" max="7" width="13.625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
         <v>49</v>
       </c>
@@ -1043,7 +1717,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:7">
       <c r="A2" t="s">
         <v>54</v>
       </c>
@@ -1066,7 +1740,7 @@
         <v>295.44</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:7">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -1089,7 +1763,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -1112,7 +1786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="6:7">
       <c r="F5" s="1" t="s">
         <v>4</v>
       </c>
@@ -1121,5 +1795,137 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="21.25" customWidth="1"/>
+    <col min="2" max="2" width="19.0625" customWidth="1"/>
+    <col min="3" max="3" width="48" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>19696.32</v>
+      </c>
+    </row>
+    <row r="3" spans="4:5">
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>19696.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="21.25" customWidth="1"/>
+    <col min="2" max="2" width="19.0625" customWidth="1"/>
+    <col min="3" max="3" width="58.0625" customWidth="1"/>
+    <col min="5" max="5" width="13.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>19696.32</v>
+      </c>
+    </row>
+    <row r="3" spans="4:5">
+      <c r="D3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="1">
+        <v>19696.32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added rb types 15, 16, 17
</commit_message>
<xml_diff>
--- a/files/reports/rb/rb_report.xlsx
+++ b/files/reports/rb/rb_report.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011" filterPrivacy="true"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="8010" windowWidth="14805" xWindow="0" yWindow="0"/>
+    <workbookView windowWidth="28800" windowHeight="13940"/>
   </bookViews>
   <sheets>
-    <sheet name="Итог" sheetId="2" r:id="rId4"/>
-    <sheet name="Скидка  на группы товаров" sheetId="3" r:id="rId6"/>
-    <sheet name="Скидка за представленность" sheetId="4" r:id="rId7"/>
-    <sheet name="Скидка на МТЗ" sheetId="5" r:id="rId8"/>
-    <sheet name="Скидка за выполнение плана прод" sheetId="6" r:id="rId9"/>
-    <sheet name="Скидка РБ по логистике" sheetId="7" r:id="rId10"/>
-    <sheet name="Скидка РБ объем за закупку в пр" sheetId="8" r:id="rId11"/>
-    <sheet name="Скидка  РБ за прирост продаж" sheetId="9" r:id="rId12"/>
+    <sheet name="Итог" sheetId="2" r:id="rId1"/>
+    <sheet name="Скидка  на группы товаров" sheetId="3" r:id="rId2"/>
+    <sheet name="Скидка за представленность" sheetId="4" r:id="rId3"/>
+    <sheet name="Скидка на МТЗ" sheetId="5" r:id="rId4"/>
+    <sheet name="Скидка за выполнение плана прод" sheetId="6" r:id="rId5"/>
+    <sheet name="Скидка РБ по логистике" sheetId="7" r:id="rId6"/>
+    <sheet name="Скидка РБ объем за закупку в пр" sheetId="8" r:id="rId7"/>
+    <sheet name="Скидка  РБ за прирост продаж" sheetId="9" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33">
   <si>
     <t>Бренд</t>
   </si>
@@ -125,16 +125,173 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:ap="http://schemas.openxmlformats.org/officeDocument/2006/extended-properties" xmlns:op="http://schemas.openxmlformats.org/officeDocument/2006/custom-properties" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cdr="http://schemas.openxmlformats.org/drawingml/2006/chartDrawing" xmlns:comp="http://schemas.openxmlformats.org/drawingml/2006/compatibility" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:lc="http://schemas.openxmlformats.org/drawingml/2006/lockedCanvas" xmlns:pic="http://schemas.openxmlformats.org/drawingml/2006/picture" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:sl="http://schemas.openxmlformats.org/schemaLibrary/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xne="http://schemas.microsoft.com/office/excel/2006/main" xmlns:mso="http://schemas.microsoft.com/office/2006/01/customui" xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:cppr="http://schemas.microsoft.com/office/2006/coverPageProps" xmlns:cdip="http://schemas.microsoft.com/office/2006/customDocumentInformationPanel" xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ntns="http://schemas.microsoft.com/office/2006/metadata/customXsn" xmlns:lp="http://schemas.microsoft.com/office/2006/metadata/longProperties" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" xmlns:msink="http://schemas.microsoft.com/ink/2010/main" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" xmlns:cdr14="http://schemas.microsoft.com/office/drawing/2010/chartDrawing" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns:pic14="http://schemas.microsoft.com/office/drawing/2010/picture" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:mso14="http://schemas.microsoft.com/office/2009/07/customui" xmlns:dgm14="http://schemas.microsoft.com/office/drawing/2010/diagram" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x12ac="http://schemas.microsoft.com/office/spreadsheetml/2011/1/ac" xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" xmlns:xr4="http://schemas.microsoft.com/office/spreadsheetml/2016/revision4" xmlns:xr5="http://schemas.microsoft.com/office/spreadsheetml/2016/revision5" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr7="http://schemas.microsoft.com/office/spreadsheetml/2016/revision7" xmlns:xr8="http://schemas.microsoft.com/office/spreadsheetml/2016/revision8" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr11="http://schemas.microsoft.com/office/spreadsheetml/2016/revision11" xmlns:xr12="http://schemas.microsoft.com/office/spreadsheetml/2016/revision12" xmlns:xr13="http://schemas.microsoft.com/office/spreadsheetml/2016/revision13" xmlns:xr14="http://schemas.microsoft.com/office/spreadsheetml/2016/revision14" xmlns:xr15="http://schemas.microsoft.com/office/spreadsheetml/2016/revision15" xmlns:x16="http://schemas.microsoft.com/office/spreadsheetml/2014/11/main" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:mo="http://schemas.microsoft.com/office/mac/office/2008/main" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:o="urn:schemas-microsoft-com:office:office" xmlns:v="urn:schemas-microsoft-com:vml" mc:Ignorable="c14 cdr14 a14 pic14 x14 xdr14 x14ac dsp mso14 dgm14 x15 x12ac x15ac xr xr2 xr3 xr4 xr5 xr6 xr7 xr8 xr9 xr10 xr11 xr12 xr13 xr14 xr15 x15 x16 x16r2 mo mx mv o v" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -144,10 +301,197 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF5DEB3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -170,21 +514,313 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="true" applyBorder="true" applyAlignment="false">
-      <alignment/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="Accent2" xfId="16" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="17" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="18" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="19" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="20" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32"/>
+    <cellStyle name="Bad" xfId="22" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="23" builtinId="42"/>
+    <cellStyle name="Total" xfId="24" builtinId="25"/>
+    <cellStyle name="Output" xfId="25" builtinId="21"/>
+    <cellStyle name="Currency" xfId="26" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38"/>
+    <cellStyle name="Note" xfId="28" builtinId="10"/>
+    <cellStyle name="Input" xfId="29" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="30" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="31" builtinId="22"/>
+    <cellStyle name="Good" xfId="32" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="33" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="34" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="35" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="36" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="37" builtinId="50"/>
+    <cellStyle name="Title" xfId="38" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="39" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="40" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="41" builtinId="9"/>
+    <cellStyle name="20% - Accent2" xfId="42" builtinId="34"/>
+    <cellStyle name="Link" xfId="43" builtinId="8"/>
+    <cellStyle name="Heading 2" xfId="44" builtinId="17"/>
+    <cellStyle name="Comma" xfId="45" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="46" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="47" builtinId="40"/>
+    <cellStyle name="Percent" xfId="48" builtinId="5"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -231,7 +867,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -266,7 +902,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -440,29 +1076,25 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="true" workbookViewId="0"/>
-  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="5"/>
+  <cols>
+    <col min="5" max="5" width="11.375" customWidth="1"/>
+    <col min="6" max="6" width="10.5625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -482,7 +1114,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>6</v>
       </c>
@@ -490,7 +1122,7 @@
         <v>7</v>
       </c>
       <c r="D2">
-        <v>286.3574438202247</v>
+        <v>286.357443820225</v>
       </c>
       <c r="E2">
         <v>1424</v>
@@ -499,7 +1131,7 @@
         <v>407773</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -516,7 +1148,7 @@
         <v>8760</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -529,17 +1161,89 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>646.8</v>
+      </c>
+    </row>
+    <row r="3" spans="4:6">
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="3" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -550,56 +1254,38 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>646.8</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="D3" s="1"/>
-      <c r="E3" s="1" t="s">
+    <row r="4" spans="4:5">
+      <c r="D4" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="1" t="s">
-        <v>18</v>
+      <c r="E4" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -610,34 +1296,122 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4">
-      <c r="D4" s="1" t="s">
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>485.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4">
+        <v>10</v>
+      </c>
+      <c r="F4">
+        <v>139.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5">
         <v>5</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6">
+      <c r="D6" s="1"/>
+      <c r="E6" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="5" outlineLevelCol="5"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -657,35 +1431,35 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
+        <v>69.75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>17</v>
@@ -697,7 +1471,7 @@
         <v>485.1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -705,59 +1479,65 @@
         <v>22</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>23</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="F4">
-        <v>139.5</v>
-      </c>
-    </row>
-    <row r="5">
+        <v>251.1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C5" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
       </c>
       <c r="E5">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="6" spans="4:6">
       <c r="D6" s="1"/>
       <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="6" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -768,116 +1548,38 @@
         <v>11</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>0</v>
+        <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E2">
+    <row r="7" spans="4:5">
+      <c r="D7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F2">
-        <v>69.75</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3">
-        <v>9</v>
-      </c>
-      <c r="F3">
-        <v>485.1</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4">
-        <v>18</v>
-      </c>
-      <c r="F4">
-        <v>251.1</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5">
-        <v>10</v>
-      </c>
-      <c r="F5">
-        <v>539</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="D6" s="1"/>
-      <c r="E6" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
+      <c r="E7" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="4" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -894,31 +1596,83 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2"/>
-    <row r="3"/>
-    <row r="4"/>
-    <row r="5"/>
-    <row r="6"/>
-    <row r="7">
-      <c r="D7" s="1" t="s">
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2">
         <v>5</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
+      <c r="E2">
+        <v>22323.05</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>31252.27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4">
+        <v>9</v>
+      </c>
+      <c r="E4">
+        <v>40181.49</v>
+      </c>
+    </row>
+    <row r="5" spans="4:5">
+      <c r="D5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
+  <sheetFormatPr defaultColWidth="8.4375" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="4"/>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>2</v>
       </c>
@@ -935,98 +1689,11 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:5">
       <c r="A2" t="s">
         <v>14</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <v>22323.05</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3">
-        <v>7</v>
-      </c>
-      <c r="E3">
-        <v>31252.27</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>40181.49</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="D5" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-  </sheetData>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" t="s">
         <v>31</v>
       </c>
       <c r="C2" t="s">
@@ -1039,7 +1706,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="4:5">
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
@@ -1048,5 +1715,7 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>